<commit_message>
Update app, add 2022 data, clean 2022 data
</commit_message>
<xml_diff>
--- a/data/tower_count/tower_count_2020.xlsx
+++ b/data/tower_count/tower_count_2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejgna\Documents\project-eleanor-and-wriley\data\tower_count\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C43FB3C5-6421-4390-8ED7-5389B07FEC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946CA76E-54F2-4515-848D-32C69CADEC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{2859B217-D451-4C41-B309-B0BCD1CFC6A4}"/>
   </bookViews>
@@ -463,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F30AE9-C51B-4D15-8ACD-A76DA395D501}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>